<commit_message>
(CENSORED data) Updated wy2016-17 Outflow pMeHg  folder;  Updated pMeHg model results file for wy2016-17;  Updated the Outflow Q and WQ worksheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Sites/Outflow_11452900/1_wy2016_2017/1_rloadest/1_pMeHg/1_Excel for Text Files/pMeHg_Comb_OutletR.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Sites/Outflow_11452900/1_wy2016_2017/1_rloadest/1_pMeHg/1_Excel for Text Files/pMeHg_Comb_OutletR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Sites\Outflow_11452900\1_wy2016_2017\1_rloadest\1_pMeHg\1_Excel for Text Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA4144C-7852-49F0-8D87-131F6F328598}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B309C50-C4CF-48FB-8B50-757429D863F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12270" xr2:uid="{B03B121B-3D8D-434D-8A7D-1765BA092E34}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12270" xr2:uid="{AA14F68A-005E-40C3-89E1-28C4D3A78C7E}"/>
   </bookViews>
   <sheets>
     <sheet name="pMeHg_Comb" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Dates</t>
   </si>
@@ -36,10 +36,7 @@
     <t>Flow</t>
   </si>
   <si>
-    <t>PpMeHg</t>
-  </si>
-  <si>
-    <t>RpMeHg</t>
+    <t>pMeHg</t>
   </si>
   <si>
     <t>10d</t>
@@ -49,12 +46,6 @@
   </si>
   <si>
     <t>6n</t>
-  </si>
-  <si>
-    <t>2s</t>
-  </si>
-  <si>
-    <t>&lt;</t>
   </si>
   <si>
     <t>14:20</t>
@@ -112,8 +103,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -430,14 +423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BE89AA-56BB-454E-8856-43F4945BD7C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490C8C07-679C-42A9-8E65-63621929E08B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +438,7 @@
     <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,28 +451,22 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42389</v>
       </c>
@@ -493,7 +480,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42392</v>
       </c>
@@ -504,13 +491,10 @@
         <v>58</v>
       </c>
       <c r="D4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42393</v>
       </c>
@@ -521,13 +505,10 @@
         <v>114</v>
       </c>
       <c r="D5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42402</v>
       </c>
@@ -541,7 +522,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42403</v>
       </c>
@@ -555,7 +536,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42404</v>
       </c>
@@ -569,7 +550,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42436</v>
       </c>
@@ -583,12 +564,12 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42437</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>551</v>
@@ -597,7 +578,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42438</v>
       </c>
@@ -611,7 +592,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42439</v>
       </c>
@@ -625,7 +606,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42441</v>
       </c>
@@ -639,7 +620,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42442</v>
       </c>
@@ -653,7 +634,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42443</v>
       </c>
@@ -663,11 +644,11 @@
       <c r="C15">
         <v>3176</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42444</v>
       </c>

</xml_diff>